<commit_message>
Spannungswandler geändert. Stückliste aktualisiert.
</commit_message>
<xml_diff>
--- a/Schrankbeleuchtung.xlsx
+++ b/Schrankbeleuchtung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/703fe33a62fd6900/Dokumente/KiCad/Schrankbeleuchtung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/703fe33a62fd6900/Dokumente/Projekte/Schrankbeleuchtung/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{50BDA3B7-1EAA-4DF5-9900-E589E1F0AFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE045AE9-6DC7-44E0-8F09-1D214C5DE1D0}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{50BDA3B7-1EAA-4DF5-9900-E589E1F0AFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B13587D-13EE-4C01-88EE-D2635CD7E2F6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3309C108-E2F1-4EAD-AA1A-3A09F05B2433}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
   <si>
     <t>Reference</t>
   </si>
@@ -50,12 +50,6 @@
     <t>RaspberryPi_Pico</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SS34</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -80,18 +74,12 @@
     <t>100R</t>
   </si>
   <si>
-    <t>R5,R6,R7,R8</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>LM2596S-5</t>
-  </si>
-  <si>
     <t>Part No</t>
   </si>
   <si>
@@ -104,9 +92,6 @@
     <t>SC0918</t>
   </si>
   <si>
-    <t>512-SS34</t>
-  </si>
-  <si>
     <t>RQ73C2A100RBTD</t>
   </si>
   <si>
@@ -119,12 +104,6 @@
     <t>ERA-6APB103V</t>
   </si>
   <si>
-    <t>LM2596SX-5.0NOPB</t>
-  </si>
-  <si>
-    <t>926-LM2596SX-5.0NOPB</t>
-  </si>
-  <si>
     <t>710-694106301002</t>
   </si>
   <si>
@@ -143,27 +122,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>100µF</t>
-  </si>
-  <si>
-    <t>81-GRM32ER61A107ME0L</t>
-  </si>
-  <si>
-    <t>GRM32ER61A107ME0L</t>
-  </si>
-  <si>
-    <t>SPM7054VC-330M-D</t>
-  </si>
-  <si>
-    <t>810-SPM7054VC-330M-D</t>
-  </si>
-  <si>
-    <t>667-EEE-FKE101XAL</t>
-  </si>
-  <si>
-    <t>EEE-FKE101XAL</t>
-  </si>
-  <si>
     <t>Price / Pice</t>
   </si>
   <si>
@@ -200,9 +158,6 @@
     <t>Pins</t>
   </si>
   <si>
-    <t>710-61302011121</t>
-  </si>
-  <si>
     <t>A1'</t>
   </si>
   <si>
@@ -213,16 +168,143 @@
   </si>
   <si>
     <t xml:space="preserve">Schablone </t>
+  </si>
+  <si>
+    <t>81-GRM21BZ71E106KE5K</t>
+  </si>
+  <si>
+    <t>GRM21BZ71E106KE5K</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>22µF</t>
+  </si>
+  <si>
+    <t>81-GRM21BZ71A226ME5L</t>
+  </si>
+  <si>
+    <t>GRM21BZ71A226ME5L</t>
+  </si>
+  <si>
+    <t>0.1µF</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>581-0805ZC104JAT2A</t>
+  </si>
+  <si>
+    <t>0805ZC104JAT2A</t>
+  </si>
+  <si>
+    <t>81-LQH44PN100MPRL</t>
+  </si>
+  <si>
+    <t>LQH44PN100MPRL</t>
+  </si>
+  <si>
+    <t>R5,R6,R7,R8,R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>3.16k</t>
+  </si>
+  <si>
+    <t>603-NT0805DRD073K16L</t>
+  </si>
+  <si>
+    <t>NT0805DRD073K16L</t>
+  </si>
+  <si>
+    <t>595-TPS560430XDBVT</t>
+  </si>
+  <si>
+    <t>TPS560430XDBVT</t>
+  </si>
+  <si>
+    <t>649-68000-220HLF</t>
+  </si>
+  <si>
+    <t>68000-220HLF</t>
+  </si>
+  <si>
+    <t>Order No</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>2648-SC0918CT-ND</t>
+  </si>
+  <si>
+    <t>490-GRM21BZ71E106KE15LCT-ND</t>
+  </si>
+  <si>
+    <t>490-GRM21BZ71A226ME15LCT-ND</t>
+  </si>
+  <si>
+    <t>478-KGM21NR71A104JTCT-ND</t>
+  </si>
+  <si>
+    <t>732-5930-ND</t>
+  </si>
+  <si>
+    <t>455-B2B-XH-AM-ND</t>
+  </si>
+  <si>
+    <t>118-SRN4018BTA-100MCT-ND</t>
+  </si>
+  <si>
+    <t>IRLML6344TRPBFCT-ND</t>
+  </si>
+  <si>
+    <t>A140898CT-ND</t>
+  </si>
+  <si>
+    <t>P10KAZCT-ND</t>
+  </si>
+  <si>
+    <t>13-NT0805DRD073K16LCT-ND</t>
+  </si>
+  <si>
+    <t>296-TPS560430XDBVTCT-ND</t>
+  </si>
+  <si>
+    <t>1 St</t>
+  </si>
+  <si>
+    <t>1St</t>
+  </si>
+  <si>
+    <t>Versand</t>
+  </si>
+  <si>
+    <t>455-2266-ND</t>
+  </si>
+  <si>
+    <t>455-1042-100-ND</t>
+  </si>
+  <si>
+    <t>609-5100-ND</t>
+  </si>
+  <si>
+    <t>10 St</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +435,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -699,7 +787,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,8 +795,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1088,459 +1179,794 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0DAE75-4450-432B-A5FB-7230BEC7406A}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" customWidth="1"/>
     <col min="6" max="7" width="11.5546875" style="3"/>
+    <col min="8" max="8" width="29.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2*B2</f>
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>34</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3">
-        <v>0.66</v>
+        <v>5.7</v>
       </c>
       <c r="G3" s="3">
         <f>F3*B3</f>
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.7</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="J3" s="3">
+        <f>I3*B3</f>
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3">
-        <v>0.69</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G12" si="0">F4*B4</f>
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G4:G5" si="0">F4*B4</f>
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J14" si="1">I4*B4</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F5" s="3">
-        <v>0.43</v>
+        <v>0.27</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6*B6</f>
+        <v>0.27</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:G14" si="2">F7*B7</f>
+        <v>0.87</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.88</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="0"/>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" si="0"/>
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
+      <c r="C10" t="s">
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
       </c>
       <c r="F10" s="3">
-        <v>0.43</v>
+        <v>0.32</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>1.72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1.28</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.72</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="5">
+        <f>SUM(G3:G14)</f>
+        <v>15.090999999999999</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="5">
+        <f>SUM(J3:J14)</f>
+        <v>15.560000000000002</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="5">
+        <v>129.65</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="5">
+        <v>133.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
+      <c r="F19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <f>B8</f>
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="3">
+        <f>F20*B20</f>
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="J20" s="3">
+        <f>I20*B20</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="3">
+        <f>F21*B21</f>
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2.21</v>
+      </c>
+      <c r="J21" s="3">
+        <f>I21</f>
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22*B22</f>
+        <v>2.08</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" ref="J22" si="3">I22*B22</f>
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G24" s="5">
+        <f>SUM(G20:G22)</f>
+        <v>3.68</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="5">
+        <f>SUM(J20:J22)</f>
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G25" s="5">
+        <v>24.2</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="5">
+        <v>24.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G27" s="5">
+        <f>G24+G16</f>
+        <v>18.771000000000001</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5">
+        <f>J24+J16</f>
+        <v>20.730000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G28" s="5">
+        <f>G25+G17</f>
+        <v>153.85</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5">
+        <f>J25+J17</f>
+        <v>157.97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="3">
-        <v>5.47</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="0"/>
-        <v>5.47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" s="6">
-        <f>SUM(G2:G12)</f>
-        <v>21.169999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="F33" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="G33" s="3">
+        <f>F33*B33</f>
+        <v>14.8</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17">
-        <f>B7</f>
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G17" s="3">
-        <f>F17*B17</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="3">
-        <f>F18*B18</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19">
-        <v>61302011121</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1.19</v>
-      </c>
-      <c r="G19" s="3">
-        <f>F19*B19</f>
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="6">
-        <f>SUM(G17:G19)</f>
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>14.8</v>
-      </c>
-      <c r="G23" s="3">
-        <f>F23*B23</f>
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="F34" s="3">
         <v>9.9</v>
       </c>
-      <c r="G24" s="3">
-        <f>F24*B24</f>
+      <c r="G34" s="3">
+        <f>F34*B34</f>
         <v>9.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G26" s="6">
-        <f>SUM(G23:G24)</f>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G36" s="5">
+        <f>SUM(G33:G34)</f>
         <v>24.700000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G28" s="3">
-        <f>SUM(G26,G21,G14)</f>
-        <v>49.85</v>
-      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G38" s="3">
+        <f>SUM(G36,G24)</f>
+        <v>28.380000000000003</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>